<commit_message>
Updated a test suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/FTP/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/FTP/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
@@ -53,9 +53,6 @@
     <t>Percentage Automated:</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>NextAndBackButtonStates</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>Automated</t>
+  </si>
+  <si>
+    <t>Finished</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")+COUNTIF($D:$D,"Testing")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1">
         <v>8</v>
@@ -600,19 +600,19 @@
         <v>8</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="6">
         <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -621,23 +621,23 @@
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -653,7 +653,7 @@
       </c>
       <c r="G5" s="3">
         <f>SUM($B:$B)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.44444444444444442</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>